<commit_message>
Completed Reddit and Western Union
</commit_message>
<xml_diff>
--- a/Emerging Tech/SYM_MODEL.xlsx
+++ b/Emerging Tech/SYM_MODEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Emerging Tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206B6C0F-8AF6-49A9-8E89-68D2AE2FF309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52F1562-4F88-434D-A25B-3108908C5DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9885" yWindow="7665" windowWidth="21600" windowHeight="11385" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -879,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB11C10-986F-41A4-B3DD-2A72A923BC11}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -3325,21 +3325,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -3483,31 +3468,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3523,4 +3499,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>